<commit_message>
Einde komt in zicht
</commit_message>
<xml_diff>
--- a/CASE_E_INPUT.xlsx
+++ b/CASE_E_INPUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axwau\Documents\caseEibmcplex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789E64D-B211-40F4-B4B8-4E4C20DE2616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360CE5CA-3F17-4D01-8921-A9C7F4739EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6680" yWindow="0" windowWidth="12610" windowHeight="10170" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual" sheetId="45" r:id="rId1"/>
@@ -2468,7 +2468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610B96D7-1082-46EC-950D-18F4EAFC725D}">
   <dimension ref="A1:EM32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A32"/>
     </sheetView>
   </sheetViews>
@@ -16275,8 +16275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="61" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16513,8 +16513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AD101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21585,8 +21585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B27"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22833,8 +22833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23348,7 +23348,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>